<commit_message>
M3 QA Cord #523 - Update excel export   - COA 5
</commit_message>
<xml_diff>
--- a/05.Controls/M3.QA.Controls/Resources/Excels/COA3.xlsx
+++ b/05.Controls/M3.QA.Controls/Resources/Excels/COA3.xlsx
@@ -779,6 +779,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -796,33 +823,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -957,7 +957,7 @@
         <xdr:cNvPr id="2" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2D4566D-82C7-43B4-8F00-5DB3CEE09EA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D2D4566D-82C7-43B4-8F00-5DB3CEE09EA6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -969,7 +969,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -992,14 +992,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1305,7 +1305,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1315,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:I14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5546875" defaultRowHeight="13.2"/>
@@ -2051,7 +2051,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="M7" s="67"/>
+      <c r="M7" s="76"/>
     </row>
     <row r="8" spans="1:20" ht="20.399999999999999">
       <c r="A8" s="1"/>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="8"/>
-      <c r="M8" s="67"/>
+      <c r="M8" s="76"/>
     </row>
     <row r="9" spans="1:20" ht="19.8">
       <c r="A9" s="1"/>
@@ -2080,18 +2080,18 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:20" ht="26.4">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="68"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
     </row>
     <row r="11" spans="1:20" ht="19.8">
       <c r="A11" s="1"/>
@@ -2113,10 +2113,10 @@
       <c r="D12" s="9"/>
       <c r="E12" s="1"/>
       <c r="F12" s="37"/>
-      <c r="G12" s="69" t="s">
+      <c r="G12" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="69"/>
+      <c r="H12" s="78"/>
       <c r="I12" s="24"/>
       <c r="J12" s="10" t="s">
         <v>8</v>
@@ -2135,13 +2135,13 @@
       <c r="H13" s="83"/>
       <c r="I13" s="84"/>
       <c r="J13" s="38"/>
-      <c r="N13" s="70"/>
-      <c r="O13" s="70"/>
-      <c r="P13" s="70"/>
-      <c r="Q13" s="70"/>
-      <c r="R13" s="70"/>
-      <c r="S13" s="70"/>
-      <c r="T13" s="70"/>
+      <c r="N13" s="79"/>
+      <c r="O13" s="79"/>
+      <c r="P13" s="79"/>
+      <c r="Q13" s="79"/>
+      <c r="R13" s="79"/>
+      <c r="S13" s="79"/>
+      <c r="T13" s="79"/>
     </row>
     <row r="14" spans="1:20" ht="22.5" customHeight="1">
       <c r="A14" s="9" t="s">
@@ -2165,14 +2165,14 @@
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="71" t="s">
+      <c r="F15" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="72"/>
-      <c r="H15" s="71" t="s">
+      <c r="G15" s="81"/>
+      <c r="H15" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="72"/>
+      <c r="I15" s="81"/>
       <c r="J15" s="41" t="s">
         <v>13</v>
       </c>
@@ -2218,27 +2218,27 @@
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:14" ht="19.8">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="79" t="s">
+      <c r="B19" s="70"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="79" t="s">
+      <c r="E19" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="79" t="s">
+      <c r="F19" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="79" t="s">
+      <c r="G19" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="H19" s="73" t="s">
+      <c r="H19" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="73" t="s">
+      <c r="I19" s="67" t="s">
         <v>19</v>
       </c>
       <c r="J19" s="47" t="s">
@@ -2246,15 +2246,15 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="21.6">
-      <c r="A20" s="76"/>
-      <c r="B20" s="77"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="76"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="68"/>
       <c r="J20" s="48" t="s">
         <v>21</v>
       </c>
@@ -2500,11 +2500,11 @@
       <c r="C33" s="66"/>
       <c r="D33" s="66"/>
       <c r="E33" s="66"/>
-      <c r="H33" s="81" t="s">
+      <c r="H33" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="I33" s="81"/>
-      <c r="J33" s="81"/>
+      <c r="I33" s="69"/>
+      <c r="J33" s="69"/>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1">
       <c r="M34" s="2"/>
@@ -2671,6 +2671,13 @@
     <protectedRange sqref="E11" name="Range1"/>
   </protectedRanges>
   <mergeCells count="15">
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="F13:I14"/>
     <mergeCell ref="I19:I20"/>
     <mergeCell ref="H33:J33"/>
     <mergeCell ref="H19:H20"/>
@@ -2679,13 +2686,6 @@
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:G20"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="F13:I14"/>
   </mergeCells>
   <conditionalFormatting sqref="E21">
     <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="notBetween">

</xml_diff>